<commit_message>
Table des transitions de l'automate complétée
</commit_message>
<xml_diff>
--- a/transitions.xlsx
+++ b/transitions.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsauget/Documents/INSA/4IF/grammaire/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="107">
   <si>
     <t>var</t>
   </si>
@@ -787,7 +782,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -798,18 +793,18 @@
   <dimension ref="A1:AD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="26" width="5.83203125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="26" width="5.875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -893,7 +888,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>26</v>
       </c>
@@ -934,7 +929,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
@@ -978,7 +973,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>
@@ -1015,7 +1010,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
@@ -1043,7 +1038,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>29</v>
       </c>
@@ -1074,7 +1069,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
@@ -1105,7 +1100,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>31</v>
       </c>
@@ -1133,7 +1128,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>32</v>
       </c>
@@ -1161,7 +1156,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>33</v>
       </c>
@@ -1202,7 +1197,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>34</v>
       </c>
@@ -1230,7 +1225,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -1286,7 +1281,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>36</v>
       </c>
@@ -1294,8 +1289,12 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1312,25 +1311,56 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="5"/>
+      <c r="B14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q14" s="3"/>
       <c r="AC14" s="1" t="s">
         <v>77</v>
       </c>
@@ -1338,7 +1368,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
@@ -1346,8 +1376,12 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1364,7 +1398,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>39</v>
       </c>
@@ -1375,7 +1409,9 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -1390,25 +1426,56 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="5"/>
+      <c r="B17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q17" s="3"/>
       <c r="AC17" s="6" t="s">
         <v>81</v>
       </c>
@@ -1416,25 +1483,56 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="5"/>
+      <c r="B18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="3"/>
       <c r="AC18" s="1" t="s">
         <v>82</v>
       </c>
@@ -1442,7 +1540,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>42</v>
       </c>
@@ -1451,14 +1549,18 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="P19" s="5"/>
       <c r="AC19" s="6" t="s">
@@ -1468,7 +1570,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>43</v>
       </c>
@@ -1477,15 +1579,23 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="K20" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="N20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="P20" s="5"/>
       <c r="AC20" s="1" t="s">
         <v>84</v>
@@ -1494,25 +1604,56 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="5"/>
+      <c r="B21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q21" s="3"/>
       <c r="AC21" s="6" t="s">
         <v>85</v>
       </c>
@@ -1520,7 +1661,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>45</v>
       </c>
@@ -1532,58 +1673,135 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="L22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="5"/>
+      <c r="X22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="AC22" s="1"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="5"/>
+      <c r="B23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q23" s="3"/>
       <c r="AC23" s="6"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="5"/>
+      <c r="B24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q24" s="3"/>
       <c r="AC24" s="1"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>48</v>
       </c>
@@ -1595,16 +1813,31 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="L25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="5"/>
+      <c r="X25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="AC25" s="6"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>49</v>
       </c>
@@ -1618,14 +1851,16 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
+      <c r="L26" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="5"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>50</v>
       </c>
@@ -1639,13 +1874,15 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
+      <c r="L27" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>51</v>
       </c>
@@ -1660,12 +1897,14 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>52</v>
       </c>
@@ -1677,15 +1916,27 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="L29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="5"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="Y29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>53</v>
       </c>
@@ -1697,15 +1948,24 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="L30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="5"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="Z30" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>54</v>
       </c>
@@ -1718,14 +1978,18 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="K31" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="N31" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="O31" s="4"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>55</v>
       </c>
@@ -1734,38 +1998,73 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="N32" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="O32" s="4"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="5"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>57</v>
       </c>
@@ -1776,7 +2075,9 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -1785,27 +2086,58 @@
       <c r="O34" s="4"/>
       <c r="P34" s="5"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="5"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q35" s="3"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>59</v>
       </c>
@@ -1814,58 +2146,128 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="K36" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
+      <c r="N36" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="5"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q37" s="3"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="5"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q38" s="3"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>62</v>
       </c>
@@ -1880,30 +2282,62 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="M39" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="5"/>
+      <c r="B40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Validation automate + table des transitions Benharkat
</commit_message>
<xml_diff>
--- a/transitions.xlsx
+++ b/transitions.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsauget/Documents/INSA/4IF/grammaire/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="107">
   <si>
     <t>var</t>
   </si>
@@ -363,7 +368,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -465,11 +470,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -511,6 +578,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -782,7 +867,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -793,15 +878,15 @@
   <dimension ref="A1:AD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="26" width="5.875" style="2" customWidth="1"/>
-    <col min="29" max="29" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="26" width="5.83203125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="5.83203125" customWidth="1"/>
+    <col min="30" max="30" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -892,36 +977,45 @@
       <c r="A2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="Q2" s="15"/>
+      <c r="R2" s="16" t="s">
         <v>25</v>
       </c>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="17"/>
       <c r="AC2" s="1" t="s">
         <v>67</v>
       </c>
@@ -929,7 +1023,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
@@ -960,12 +1054,20 @@
       <c r="P3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="5"/>
       <c r="AC3" s="6" t="s">
         <v>64</v>
       </c>
@@ -1000,9 +1102,18 @@
       <c r="P4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="Q4" s="3"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="5"/>
       <c r="AC4" s="1" t="s">
         <v>68</v>
       </c>
@@ -1031,6 +1142,16 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="5"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="5"/>
       <c r="AC5" s="6" t="s">
         <v>69</v>
       </c>
@@ -1059,9 +1180,18 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="5"/>
-      <c r="T6" s="2" t="s">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="5"/>
       <c r="AC6" s="1" t="s">
         <v>70</v>
       </c>
@@ -1090,9 +1220,18 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
-      <c r="U7" s="2" t="s">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="5"/>
       <c r="AC7" s="6" t="s">
         <v>71</v>
       </c>
@@ -1121,6 +1260,16 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="5"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="5"/>
       <c r="AC8" s="1" t="s">
         <v>72</v>
       </c>
@@ -1149,6 +1298,16 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="5"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="5"/>
       <c r="AC9" s="6" t="s">
         <v>73</v>
       </c>
@@ -1181,13 +1340,20 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="5"/>
-      <c r="X10" s="2" t="s">
+      <c r="Q10" s="3"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Y10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="Z10" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AC10" s="1" t="s">
@@ -1197,7 +1363,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>34</v>
       </c>
@@ -1218,6 +1384,16 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="5"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="5"/>
       <c r="AC11" s="6" t="s">
         <v>65</v>
       </c>
@@ -1241,39 +1417,31 @@
       <c r="E12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
       <c r="P12" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="5"/>
       <c r="AC12" s="1" t="s">
         <v>75</v>
       </c>
@@ -1304,6 +1472,16 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="5"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="5"/>
       <c r="AC13" s="6" t="s">
         <v>76</v>
       </c>
@@ -1315,52 +1493,35 @@
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
         <v>71</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="5"/>
       <c r="Q14" s="3"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="5"/>
       <c r="AC14" s="1" t="s">
         <v>77</v>
       </c>
@@ -1391,6 +1552,16 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="5"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="5"/>
       <c r="AC15" s="6" t="s">
         <v>78</v>
       </c>
@@ -1419,6 +1590,16 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="5"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="5"/>
       <c r="AC16" s="1" t="s">
         <v>79</v>
       </c>
@@ -1430,52 +1611,39 @@
       <c r="A17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
       <c r="L17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="N17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="Q17" s="3"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="5"/>
       <c r="AC17" s="6" t="s">
         <v>81</v>
       </c>
@@ -1487,52 +1655,33 @@
       <c r="A18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="5"/>
       <c r="Q18" s="3"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="5"/>
       <c r="AC18" s="1" t="s">
         <v>82</v>
       </c>
@@ -1563,6 +1712,16 @@
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="5"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="5"/>
       <c r="AC19" s="6" t="s">
         <v>83</v>
       </c>
@@ -1597,6 +1756,16 @@
         <v>53</v>
       </c>
       <c r="P20" s="5"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="5"/>
       <c r="AC20" s="1" t="s">
         <v>84</v>
       </c>
@@ -1608,52 +1777,39 @@
       <c r="A21" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
       <c r="K21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
       <c r="N21" s="4" t="s">
         <v>82</v>
       </c>
       <c r="O21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="P21" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="P21" s="5"/>
       <c r="Q21" s="3"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="5"/>
       <c r="AC21" s="6" t="s">
         <v>85</v>
       </c>
@@ -1686,13 +1842,20 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="5"/>
-      <c r="X22" s="2" t="s">
+      <c r="Q22" s="3"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y22" s="2" t="s">
+      <c r="Y22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Z22" s="2" t="s">
+      <c r="Z22" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AC22" s="1"/>
@@ -1701,104 +1864,78 @@
       <c r="A23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
       <c r="N23" s="4" t="s">
         <v>84</v>
       </c>
       <c r="O23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="P23" s="5"/>
       <c r="Q23" s="3"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="5"/>
       <c r="AC23" s="6"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="L24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
         <v>85</v>
       </c>
       <c r="O24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P24" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="P24" s="5"/>
       <c r="Q24" s="3"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="5"/>
       <c r="AC24" s="1"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
@@ -1826,13 +1963,20 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="5"/>
-      <c r="X25" s="2" t="s">
+      <c r="Q25" s="3"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Y25" s="2" t="s">
+      <c r="Y25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Z25" s="2" t="s">
+      <c r="Z25" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AC25" s="6"/>
@@ -1858,6 +2002,16 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="5"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="5"/>
       <c r="AC26" s="1"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -1881,6 +2035,16 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="5"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="5"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
@@ -1903,6 +2067,16 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="5"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="5"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
@@ -1929,10 +2103,18 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="5"/>
-      <c r="Y29" s="2" t="s">
+      <c r="Q29" s="3"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Z29" s="2" t="s">
+      <c r="Z29" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1961,7 +2143,16 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="5"/>
-      <c r="Z30" s="2" t="s">
+      <c r="Q30" s="3"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1988,6 +2179,16 @@
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="5"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="5"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
@@ -2012,59 +2213,52 @@
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="5"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q32" s="3"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="5"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="P33" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="5"/>
       <c r="Q33" s="3"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="5"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>57</v>
       </c>
@@ -2085,59 +2279,52 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="5"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q34" s="3"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="5"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="M35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="O35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="P35" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="5"/>
       <c r="Q35" s="3"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="5"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>59</v>
       </c>
@@ -2164,110 +2351,94 @@
         <v>53</v>
       </c>
       <c r="P36" s="5"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q36" s="3"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="5"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
       <c r="G37" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
       <c r="K37" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
       <c r="N37" s="4" t="s">
         <v>81</v>
       </c>
       <c r="O37" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="P37" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="P37" s="5"/>
       <c r="Q37" s="3"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="5"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H38" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
       <c r="K38" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L38" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
       <c r="N38" s="4" t="s">
         <v>83</v>
       </c>
       <c r="O38" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P38" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="P38" s="5"/>
       <c r="Q38" s="3"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="5"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>62</v>
       </c>
@@ -2288,56 +2459,50 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="5"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q39" s="3"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="5"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="G40" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="O40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="P40" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correction de l'automate pour l'acceptation (état 0 et non état 2)
</commit_message>
<xml_diff>
--- a/transitions.xlsx
+++ b/transitions.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsauget/Documents/INSA/4IF/grammaire/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="107">
   <si>
     <t>var</t>
   </si>
@@ -536,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,6 +592,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,7 +865,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -878,18 +876,18 @@
   <dimension ref="A1:AD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="26" width="5.83203125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="5.83203125" customWidth="1"/>
-    <col min="30" max="30" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="26" width="5.875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="5.875" customWidth="1"/>
+    <col min="30" max="30" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -969,11 +967,11 @@
       <c r="AC1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>26</v>
       </c>
@@ -1004,7 +1002,9 @@
       <c r="P2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="15"/>
+      <c r="Q2" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="R2" s="16" t="s">
         <v>25</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="4"/>
@@ -1121,7 +1121,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>29</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>31</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>32</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>33</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>34</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>36</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>39</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>40</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>41</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>42</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>43</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>44</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>45</v>
       </c>
@@ -1860,7 +1860,7 @@
       </c>
       <c r="AC22" s="1"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>46</v>
       </c>
@@ -1899,7 +1899,7 @@
       <c r="Z23" s="5"/>
       <c r="AC23" s="6"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>47</v>
       </c>
@@ -1938,7 +1938,7 @@
       <c r="Z24" s="5"/>
       <c r="AC24" s="1"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>48</v>
       </c>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="AC25" s="6"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>49</v>
       </c>
@@ -2014,7 +2014,7 @@
       <c r="Z26" s="5"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>50</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="Y27" s="4"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>51</v>
       </c>
@@ -2078,7 +2078,7 @@
       <c r="Y28" s="4"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>52</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>53</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>54</v>
       </c>
@@ -2362,7 +2362,7 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="5"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>60</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="5"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>61</v>
       </c>
@@ -2438,7 +2438,7 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="5"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>62</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="Y39" s="4"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>63</v>
       </c>

</xml_diff>